<commit_message>
actualización del estado del subproyecto en Ejercicios
</commit_message>
<xml_diff>
--- a/DOCUMENTOS/Notas.xlsx
+++ b/DOCUMENTOS/Notas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\CursoHTML\DOCUMENTOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42043C64-4E69-4C77-8939-DF9B6CA9CF43}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D05D4FF0-3289-4976-9FFF-BFF97291EF59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B5A71190-DD5F-4F72-81CA-D2CDA1BEEC63}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>UF1</t>
   </si>
@@ -48,9 +48,6 @@
     <t>UF3</t>
   </si>
   <si>
-    <t>UF5</t>
-  </si>
-  <si>
     <t>Teoria</t>
   </si>
   <si>
@@ -60,9 +57,6 @@
     <t>Media</t>
   </si>
   <si>
-    <t>Media Total:</t>
-  </si>
-  <si>
     <t>Alumno</t>
   </si>
   <si>
@@ -72,18 +66,9 @@
     <t>Boga Zaragoza, Maria Angeles</t>
   </si>
   <si>
-    <t>Casadi martinez, Águeda</t>
-  </si>
-  <si>
     <t>Elabdellaoui, Saida</t>
   </si>
   <si>
-    <t>MÓDULO 1</t>
-  </si>
-  <si>
-    <t>El Fallaki, María</t>
-  </si>
-  <si>
     <t>Ferrer Lozano, Jose Francisco</t>
   </si>
   <si>
@@ -108,17 +93,23 @@
     <t>Ruiz Sedano, Francisco</t>
   </si>
   <si>
-    <t>Serrano Diaz, Luz</t>
-  </si>
-  <si>
-    <t>IFCD0110 - Diciembre 2025</t>
+    <t>Serrano Diaz, Luz (baja por faltas)</t>
+  </si>
+  <si>
+    <t>IFCD0110 - CONFECCIÓN Y PUBLICACIÓN DE PÁGINAS WEB</t>
+  </si>
+  <si>
+    <t>MF0950_2 - Construcción de páginas web</t>
+  </si>
+  <si>
+    <t>"Diciembre 2025"</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -162,6 +153,14 @@
       <name val="DejaVu Sans"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="15">
     <fill>
@@ -261,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -272,6 +271,8 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -284,8 +285,7 @@
     <xf numFmtId="0" fontId="4" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -600,10 +600,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4766EE60-6A90-445E-A732-3F299E5F976E}">
-  <dimension ref="A4:K38"/>
+  <dimension ref="A1:K36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -620,69 +620,74 @@
     <col min="11" max="11" width="6.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
+    <row r="1" spans="1:11" ht="21" x14ac:dyDescent="0.4">
+      <c r="B1" s="16" t="s">
+        <v>19</v>
+      </c>
+    </row>
     <row r="4" spans="1:11" ht="18" x14ac:dyDescent="0.35">
-      <c r="B4" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="13"/>
-      <c r="K4" s="13"/>
+      <c r="B4" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
+      <c r="G4" s="15"/>
+      <c r="H4" s="15"/>
+      <c r="I4" s="15"/>
+      <c r="J4" s="15"/>
+      <c r="K4" s="15"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C5" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="11" t="s">
+      <c r="C5" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="11"/>
-      <c r="H5" s="11"/>
-      <c r="I5" s="12" t="s">
+      <c r="G5" s="13"/>
+      <c r="H5" s="13"/>
+      <c r="I5" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="B6" s="15" t="s">
-        <v>8</v>
+      <c r="B6" s="11" t="s">
+        <v>6</v>
       </c>
       <c r="C6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="E6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="F6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="1" t="s">
-        <v>6</v>
-      </c>
       <c r="I6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.3">
@@ -690,7 +695,7 @@
         <v>1</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C7" s="4">
         <v>9.5</v>
@@ -702,11 +707,15 @@
         <f>(C7+D7)/2</f>
         <v>9.75</v>
       </c>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
+      <c r="F7" s="5">
+        <v>10</v>
+      </c>
+      <c r="G7" s="5">
+        <v>10</v>
+      </c>
       <c r="H7" s="8">
         <f>(F7+G7)/2</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
@@ -720,26 +729,32 @@
         <v>2</v>
       </c>
       <c r="B8" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C8" s="4">
         <v>10</v>
       </c>
-      <c r="D8" s="4"/>
+      <c r="D8" s="4">
+        <v>8.5</v>
+      </c>
       <c r="E8" s="7">
-        <f t="shared" ref="E8:E20" si="0">(C8+D8)/2</f>
-        <v>5</v>
-      </c>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
+        <f t="shared" ref="E8:E18" si="0">(C8+D8)/2</f>
+        <v>9.25</v>
+      </c>
+      <c r="F8" s="5">
+        <v>9.5</v>
+      </c>
+      <c r="G8" s="5">
+        <v>10</v>
+      </c>
       <c r="H8" s="8">
-        <f t="shared" ref="H8:H20" si="1">(F8+G8)/2</f>
-        <v>0</v>
+        <f t="shared" ref="H8:H18" si="1">(F8+G8)/2</f>
+        <v>9.75</v>
       </c>
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="9">
-        <f t="shared" ref="K8:K20" si="2">(I8+J8)/2</f>
+        <f t="shared" ref="K8:K18" si="2">(I8+J8)/2</f>
         <v>0</v>
       </c>
     </row>
@@ -748,19 +763,27 @@
         <v>3</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
+        <v>9</v>
+      </c>
+      <c r="C9" s="4">
+        <v>5.5</v>
+      </c>
+      <c r="D9" s="4">
+        <v>7</v>
+      </c>
       <c r="E9" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+        <v>6.25</v>
+      </c>
+      <c r="F9" s="5">
+        <v>8.5</v>
+      </c>
+      <c r="G9" s="5">
+        <v>9</v>
+      </c>
       <c r="H9" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.75</v>
       </c>
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
@@ -774,23 +797,27 @@
         <v>4</v>
       </c>
       <c r="B10" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C10" s="4">
-        <v>5.5</v>
+        <v>10</v>
       </c>
       <c r="D10" s="4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E10" s="7">
         <f t="shared" si="0"/>
-        <v>6.25</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="F10" s="5">
+        <v>9.5</v>
+      </c>
+      <c r="G10" s="5">
+        <v>8.5</v>
+      </c>
       <c r="H10" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I10" s="6"/>
       <c r="J10" s="6"/>
@@ -804,19 +831,27 @@
         <v>5</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
-      </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
+        <v>11</v>
+      </c>
+      <c r="C11" s="4">
+        <v>9</v>
+      </c>
+      <c r="D11" s="4">
+        <v>9.5</v>
+      </c>
       <c r="E11" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
+        <v>9.25</v>
+      </c>
+      <c r="F11" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="G11" s="5">
+        <v>9.5</v>
+      </c>
       <c r="H11" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.5</v>
       </c>
       <c r="I11" s="6"/>
       <c r="J11" s="6"/>
@@ -830,21 +865,27 @@
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C12" s="4">
         <v>10</v>
       </c>
-      <c r="D12" s="4"/>
+      <c r="D12" s="4">
+        <v>8</v>
+      </c>
       <c r="E12" s="7">
         <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
+        <v>9</v>
+      </c>
+      <c r="F12" s="5">
+        <v>8.5</v>
+      </c>
+      <c r="G12" s="5">
+        <v>8</v>
+      </c>
       <c r="H12" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.25</v>
       </c>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
@@ -858,21 +899,27 @@
         <v>7</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C13" s="4">
-        <v>9</v>
-      </c>
-      <c r="D13" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="D13" s="4">
+        <v>10</v>
+      </c>
       <c r="E13" s="7">
         <f t="shared" si="0"/>
-        <v>4.5</v>
-      </c>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="F13" s="5">
+        <v>9.5</v>
+      </c>
+      <c r="G13" s="5">
+        <v>9.5</v>
+      </c>
       <c r="H13" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9.5</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="6"/>
@@ -886,23 +933,27 @@
         <v>8</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C14" s="4">
-        <v>10</v>
+        <v>9.5</v>
       </c>
       <c r="D14" s="4">
         <v>8</v>
       </c>
       <c r="E14" s="7">
         <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
+        <v>8.75</v>
+      </c>
+      <c r="F14" s="5">
+        <v>10</v>
+      </c>
+      <c r="G14" s="5">
+        <v>8</v>
+      </c>
       <c r="H14" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="6"/>
@@ -916,7 +967,7 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="C15" s="4">
         <v>10</v>
@@ -928,11 +979,15 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
+      <c r="F15" s="5">
+        <v>9.5</v>
+      </c>
+      <c r="G15" s="5">
+        <v>9</v>
+      </c>
       <c r="H15" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9.25</v>
       </c>
       <c r="I15" s="6"/>
       <c r="J15" s="6"/>
@@ -946,23 +1001,27 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C16" s="4">
-        <v>9.5</v>
+        <v>8.5</v>
       </c>
       <c r="D16" s="4">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E16" s="7">
         <f t="shared" si="0"/>
         <v>8.75</v>
       </c>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
+      <c r="F16" s="5">
+        <v>8.5</v>
+      </c>
+      <c r="G16" s="5">
+        <v>8</v>
+      </c>
       <c r="H16" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>8.25</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="6"/>
@@ -976,19 +1035,27 @@
         <v>11</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
+        <v>17</v>
+      </c>
+      <c r="C17" s="4">
+        <v>10</v>
+      </c>
+      <c r="D17" s="4">
+        <v>9.5</v>
+      </c>
       <c r="E17" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
+        <v>9.75</v>
+      </c>
+      <c r="F17" s="5">
+        <v>10</v>
+      </c>
+      <c r="G17" s="5">
+        <v>9.5</v>
+      </c>
       <c r="H17" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9.75</v>
       </c>
       <c r="I17" s="6"/>
       <c r="J17" s="6"/>
@@ -1002,20 +1069,22 @@
         <v>12</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C18" s="4">
-        <v>8.5</v>
-      </c>
-      <c r="D18" s="4"/>
+        <v>10</v>
+      </c>
+      <c r="D18" s="4">
+        <v>10</v>
+      </c>
       <c r="E18" s="7">
         <f t="shared" si="0"/>
-        <v>4.25</v>
+        <v>10</v>
       </c>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="8">
-        <f t="shared" si="1"/>
+        <f>(F18+G18)/2</f>
         <v>0</v>
       </c>
       <c r="I18" s="6"/>
@@ -1026,62 +1095,20 @@
       </c>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A19">
-        <v>13</v>
-      </c>
-      <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" s="4">
-        <v>10</v>
-      </c>
-      <c r="D19" s="4"/>
-      <c r="E19" s="7">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <v>14</v>
-      </c>
-      <c r="B20" t="s">
-        <v>23</v>
-      </c>
-      <c r="C20" s="4">
-        <v>10</v>
-      </c>
-      <c r="D20" s="4">
-        <v>10</v>
-      </c>
-      <c r="E20" s="7">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="8">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-      <c r="K20" s="9">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.3">
       <c r="C21" s="3"/>
@@ -1139,51 +1166,15 @@
       <c r="G27" s="3"/>
       <c r="H27" s="3"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-    </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="C29" s="3"/>
-      <c r="D29" s="3"/>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="3"/>
-    </row>
-    <row r="33" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="E33" t="s">
-        <v>3</v>
-      </c>
-      <c r="F33" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G33" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H33" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="5:8" x14ac:dyDescent="0.3">
-      <c r="H34">
-        <f>(F34+G34)/2</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="5:8" ht="21" x14ac:dyDescent="0.4">
-      <c r="F38" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="G38" s="2"/>
-      <c r="H38" s="2">
-        <f>(E7+H22+H26+H30+H34)/5</f>
-        <v>1.95</v>
-      </c>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="36" spans="6:8" ht="13.2" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>